<commit_message>
renames columns in preductions for clarity
</commit_message>
<xml_diff>
--- a/predictions/predictions_day_1.xlsx
+++ b/predictions/predictions_day_1.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/demetri/gitrepos/Euro2020/predictions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B417FFF-E0F5-FF49-AEC8-8C2A8D0FF5D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95FE5A47-3EDB-C244-8870-94E08748A5C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="19260" yWindow="6320" windowWidth="27640" windowHeight="16940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -42,15 +42,6 @@
     <t>matchday</t>
   </si>
   <si>
-    <t>A Wins</t>
-  </si>
-  <si>
-    <t>B Wins</t>
-  </si>
-  <si>
-    <t>Draw</t>
-  </si>
-  <si>
     <t>Turkey</t>
   </si>
   <si>
@@ -123,9 +114,6 @@
     <t>Germany</t>
   </si>
   <si>
-    <t>Awon</t>
-  </si>
-  <si>
     <t>score1</t>
   </si>
   <si>
@@ -138,16 +126,28 @@
     <t>LossB</t>
   </si>
   <si>
-    <t>Bwon</t>
-  </si>
-  <si>
-    <t>NeitherWon</t>
-  </si>
-  <si>
-    <t>Loss</t>
-  </si>
-  <si>
     <t>LossDraw</t>
+  </si>
+  <si>
+    <t>team1wins</t>
+  </si>
+  <si>
+    <t>team2wins</t>
+  </si>
+  <si>
+    <t>draw</t>
+  </si>
+  <si>
+    <t>team1won</t>
+  </si>
+  <si>
+    <t>team2wins2</t>
+  </si>
+  <si>
+    <t>noteamwins</t>
+  </si>
+  <si>
+    <t>loss</t>
   </si>
 </sst>
 </file>
@@ -705,24 +705,24 @@
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="team1"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="team2"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="matchday"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="A Wins"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="B Wins"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Draw"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="team1wins"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="team2wins"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="draw"/>
     <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="score1"/>
     <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="score2"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Awon"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Bwon"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="NeitherWon"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="team1won"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="team2wins2"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="noteamwins"/>
     <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="LossA" dataDxfId="1">
-      <calculatedColumnFormula>-LOG(Table2[[#This Row],[A Wins]], EXP(1))*Table2[[#This Row],[Awon]]</calculatedColumnFormula>
+      <calculatedColumnFormula>-LOG(Table2[[#This Row],[team1wins]], EXP(1))*Table2[[#This Row],[team1won]]</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="LossB">
-      <calculatedColumnFormula>-LOG(Table2[[#This Row],[B Wins]], EXP(1))*Table2[[#This Row],[Bwon]]</calculatedColumnFormula>
+      <calculatedColumnFormula>-LOG(Table2[[#This Row],[team2wins]], EXP(1))*Table2[[#This Row],[team2wins2]]</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="LossDraw">
-      <calculatedColumnFormula>-LOG(Table2[[#This Row],[Draw]], EXP(1))*Table2[[#This Row],[NeitherWon]]</calculatedColumnFormula>
+      <calculatedColumnFormula>-LOG(Table2[[#This Row],[draw]], EXP(1))*Table2[[#This Row],[noteamwins]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="Loss" dataDxfId="0">
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="loss" dataDxfId="0">
       <calculatedColumnFormula>SUM(Table2[[#This Row],[LossA]:[LossDraw]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1030,7 +1030,7 @@
   <dimension ref="A1:O13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N23" sqref="N23"/>
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1049,48 +1049,48 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>3</v>
+        <v>32</v>
       </c>
       <c r="E1" t="s">
-        <v>4</v>
+        <v>33</v>
       </c>
       <c r="F1" t="s">
-        <v>5</v>
+        <v>34</v>
       </c>
       <c r="G1" t="s">
+        <v>27</v>
+      </c>
+      <c r="H1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I1" t="s">
+        <v>35</v>
+      </c>
+      <c r="J1" t="s">
+        <v>36</v>
+      </c>
+      <c r="K1" t="s">
+        <v>37</v>
+      </c>
+      <c r="L1" t="s">
+        <v>29</v>
+      </c>
+      <c r="M1" t="s">
+        <v>30</v>
+      </c>
+      <c r="N1" t="s">
         <v>31</v>
       </c>
-      <c r="H1" t="s">
-        <v>32</v>
-      </c>
-      <c r="I1" t="s">
-        <v>30</v>
-      </c>
-      <c r="J1" t="s">
-        <v>35</v>
-      </c>
-      <c r="K1" t="s">
-        <v>36</v>
-      </c>
-      <c r="L1" t="s">
-        <v>33</v>
-      </c>
-      <c r="M1" t="s">
-        <v>34</v>
-      </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>38</v>
-      </c>
-      <c r="O1" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -1120,15 +1120,15 @@
         <v>0</v>
       </c>
       <c r="L2">
-        <f>-LOG(Table2[[#This Row],[A Wins]], EXP(1))*Table2[[#This Row],[Awon]]</f>
+        <f>-LOG(Table2[[#This Row],[team1wins]], EXP(1))*Table2[[#This Row],[team1won]]</f>
         <v>0</v>
       </c>
       <c r="M2">
-        <f>-LOG(Table2[[#This Row],[B Wins]], EXP(1))*Table2[[#This Row],[Bwon]]</f>
+        <f>-LOG(Table2[[#This Row],[team2wins]], EXP(1))*Table2[[#This Row],[team2wins2]]</f>
         <v>0.43540898448123644</v>
       </c>
       <c r="N2">
-        <f>-LOG(Table2[[#This Row],[Draw]], EXP(1))*Table2[[#This Row],[NeitherWon]]</f>
+        <f>-LOG(Table2[[#This Row],[draw]], EXP(1))*Table2[[#This Row],[noteamwins]]</f>
         <v>0</v>
       </c>
       <c r="O2">
@@ -1138,10 +1138,10 @@
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -1171,15 +1171,15 @@
         <v>1</v>
       </c>
       <c r="L3">
-        <f>-LOG(Table2[[#This Row],[A Wins]], EXP(1))*Table2[[#This Row],[Awon]]</f>
+        <f>-LOG(Table2[[#This Row],[team1wins]], EXP(1))*Table2[[#This Row],[team1won]]</f>
         <v>0</v>
       </c>
       <c r="M3">
-        <f>-LOG(Table2[[#This Row],[B Wins]], EXP(1))*Table2[[#This Row],[Bwon]]</f>
+        <f>-LOG(Table2[[#This Row],[team2wins]], EXP(1))*Table2[[#This Row],[team2wins2]]</f>
         <v>0</v>
       </c>
       <c r="N3">
-        <f>-LOG(Table2[[#This Row],[Draw]], EXP(1))*Table2[[#This Row],[NeitherWon]]</f>
+        <f>-LOG(Table2[[#This Row],[draw]], EXP(1))*Table2[[#This Row],[noteamwins]]</f>
         <v>1.5738294849667327</v>
       </c>
       <c r="O3">
@@ -1189,10 +1189,10 @@
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C4">
         <v>1</v>
@@ -1222,15 +1222,15 @@
         <v>0</v>
       </c>
       <c r="L4">
-        <f>-LOG(Table2[[#This Row],[A Wins]], EXP(1))*Table2[[#This Row],[Awon]]</f>
+        <f>-LOG(Table2[[#This Row],[team1wins]], EXP(1))*Table2[[#This Row],[team1won]]</f>
         <v>0</v>
       </c>
       <c r="M4">
-        <f>-LOG(Table2[[#This Row],[B Wins]], EXP(1))*Table2[[#This Row],[Bwon]]</f>
+        <f>-LOG(Table2[[#This Row],[team2wins]], EXP(1))*Table2[[#This Row],[team2wins2]]</f>
         <v>1.6334744902623417</v>
       </c>
       <c r="N4">
-        <f>-LOG(Table2[[#This Row],[Draw]], EXP(1))*Table2[[#This Row],[NeitherWon]]</f>
+        <f>-LOG(Table2[[#This Row],[draw]], EXP(1))*Table2[[#This Row],[noteamwins]]</f>
         <v>0</v>
       </c>
       <c r="O4">
@@ -1240,10 +1240,10 @@
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B5" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -1273,15 +1273,15 @@
         <v>0</v>
       </c>
       <c r="L5">
-        <f>-LOG(Table2[[#This Row],[A Wins]], EXP(1))*Table2[[#This Row],[Awon]]</f>
+        <f>-LOG(Table2[[#This Row],[team1wins]], EXP(1))*Table2[[#This Row],[team1won]]</f>
         <v>0.43811744038341383</v>
       </c>
       <c r="M5">
-        <f>-LOG(Table2[[#This Row],[B Wins]], EXP(1))*Table2[[#This Row],[Bwon]]</f>
+        <f>-LOG(Table2[[#This Row],[team2wins]], EXP(1))*Table2[[#This Row],[team2wins2]]</f>
         <v>0</v>
       </c>
       <c r="N5">
-        <f>-LOG(Table2[[#This Row],[Draw]], EXP(1))*Table2[[#This Row],[NeitherWon]]</f>
+        <f>-LOG(Table2[[#This Row],[draw]], EXP(1))*Table2[[#This Row],[noteamwins]]</f>
         <v>0</v>
       </c>
       <c r="O5">
@@ -1291,10 +1291,10 @@
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B6" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C6">
         <v>1</v>
@@ -1324,15 +1324,15 @@
         <v>0</v>
       </c>
       <c r="L6">
-        <f>-LOG(Table2[[#This Row],[A Wins]], EXP(1))*Table2[[#This Row],[Awon]]</f>
+        <f>-LOG(Table2[[#This Row],[team1wins]], EXP(1))*Table2[[#This Row],[team1won]]</f>
         <v>0.33128570993391293</v>
       </c>
       <c r="M6">
-        <f>-LOG(Table2[[#This Row],[B Wins]], EXP(1))*Table2[[#This Row],[Bwon]]</f>
+        <f>-LOG(Table2[[#This Row],[team2wins]], EXP(1))*Table2[[#This Row],[team2wins2]]</f>
         <v>0</v>
       </c>
       <c r="N6">
-        <f>-LOG(Table2[[#This Row],[Draw]], EXP(1))*Table2[[#This Row],[NeitherWon]]</f>
+        <f>-LOG(Table2[[#This Row],[draw]], EXP(1))*Table2[[#This Row],[noteamwins]]</f>
         <v>0</v>
       </c>
       <c r="O6">
@@ -1342,10 +1342,10 @@
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B7" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C7">
         <v>1</v>
@@ -1375,15 +1375,15 @@
         <v>0</v>
       </c>
       <c r="L7">
-        <f>-LOG(Table2[[#This Row],[A Wins]], EXP(1))*Table2[[#This Row],[Awon]]</f>
+        <f>-LOG(Table2[[#This Row],[team1wins]], EXP(1))*Table2[[#This Row],[team1won]]</f>
         <v>0.52467103058804376</v>
       </c>
       <c r="M7">
-        <f>-LOG(Table2[[#This Row],[B Wins]], EXP(1))*Table2[[#This Row],[Bwon]]</f>
+        <f>-LOG(Table2[[#This Row],[team2wins]], EXP(1))*Table2[[#This Row],[team2wins2]]</f>
         <v>0</v>
       </c>
       <c r="N7">
-        <f>-LOG(Table2[[#This Row],[Draw]], EXP(1))*Table2[[#This Row],[NeitherWon]]</f>
+        <f>-LOG(Table2[[#This Row],[draw]], EXP(1))*Table2[[#This Row],[noteamwins]]</f>
         <v>0</v>
       </c>
       <c r="O7">
@@ -1393,10 +1393,10 @@
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B8" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C8">
         <v>1</v>
@@ -1426,15 +1426,15 @@
         <v>0</v>
       </c>
       <c r="L8">
-        <f>-LOG(Table2[[#This Row],[A Wins]], EXP(1))*Table2[[#This Row],[Awon]]</f>
+        <f>-LOG(Table2[[#This Row],[team1wins]], EXP(1))*Table2[[#This Row],[team1won]]</f>
         <v>0.72309105693301734</v>
       </c>
       <c r="M8">
-        <f>-LOG(Table2[[#This Row],[B Wins]], EXP(1))*Table2[[#This Row],[Bwon]]</f>
+        <f>-LOG(Table2[[#This Row],[team2wins]], EXP(1))*Table2[[#This Row],[team2wins2]]</f>
         <v>0</v>
       </c>
       <c r="N8">
-        <f>-LOG(Table2[[#This Row],[Draw]], EXP(1))*Table2[[#This Row],[NeitherWon]]</f>
+        <f>-LOG(Table2[[#This Row],[draw]], EXP(1))*Table2[[#This Row],[noteamwins]]</f>
         <v>0</v>
       </c>
       <c r="O8">
@@ -1444,10 +1444,10 @@
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B9" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C9">
         <v>1</v>
@@ -1477,15 +1477,15 @@
         <v>0</v>
       </c>
       <c r="L9">
-        <f>-LOG(Table2[[#This Row],[A Wins]], EXP(1))*Table2[[#This Row],[Awon]]</f>
+        <f>-LOG(Table2[[#This Row],[team1wins]], EXP(1))*Table2[[#This Row],[team1won]]</f>
         <v>0</v>
       </c>
       <c r="M9">
-        <f>-LOG(Table2[[#This Row],[B Wins]], EXP(1))*Table2[[#This Row],[Bwon]]</f>
+        <f>-LOG(Table2[[#This Row],[team2wins]], EXP(1))*Table2[[#This Row],[team2wins2]]</f>
         <v>0.95191790951730615</v>
       </c>
       <c r="N9">
-        <f>-LOG(Table2[[#This Row],[Draw]], EXP(1))*Table2[[#This Row],[NeitherWon]]</f>
+        <f>-LOG(Table2[[#This Row],[draw]], EXP(1))*Table2[[#This Row],[noteamwins]]</f>
         <v>0</v>
       </c>
       <c r="O9">
@@ -1495,10 +1495,10 @@
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B10" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C10">
         <v>1</v>
@@ -1528,15 +1528,15 @@
         <v>0</v>
       </c>
       <c r="L10">
-        <f>-LOG(Table2[[#This Row],[A Wins]], EXP(1))*Table2[[#This Row],[Awon]]</f>
+        <f>-LOG(Table2[[#This Row],[team1wins]], EXP(1))*Table2[[#This Row],[team1won]]</f>
         <v>0</v>
       </c>
       <c r="M10">
-        <f>-LOG(Table2[[#This Row],[B Wins]], EXP(1))*Table2[[#This Row],[Bwon]]</f>
+        <f>-LOG(Table2[[#This Row],[team2wins]], EXP(1))*Table2[[#This Row],[team2wins2]]</f>
         <v>1.3299140276837829</v>
       </c>
       <c r="N10">
-        <f>-LOG(Table2[[#This Row],[Draw]], EXP(1))*Table2[[#This Row],[NeitherWon]]</f>
+        <f>-LOG(Table2[[#This Row],[draw]], EXP(1))*Table2[[#This Row],[noteamwins]]</f>
         <v>0</v>
       </c>
       <c r="O10">
@@ -1546,10 +1546,10 @@
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B11" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C11">
         <v>1</v>
@@ -1579,15 +1579,15 @@
         <v>1</v>
       </c>
       <c r="L11">
-        <f>-LOG(Table2[[#This Row],[A Wins]], EXP(1))*Table2[[#This Row],[Awon]]</f>
+        <f>-LOG(Table2[[#This Row],[team1wins]], EXP(1))*Table2[[#This Row],[team1won]]</f>
         <v>0</v>
       </c>
       <c r="M11">
-        <f>-LOG(Table2[[#This Row],[B Wins]], EXP(1))*Table2[[#This Row],[Bwon]]</f>
+        <f>-LOG(Table2[[#This Row],[team2wins]], EXP(1))*Table2[[#This Row],[team2wins2]]</f>
         <v>0</v>
       </c>
       <c r="N11">
-        <f>-LOG(Table2[[#This Row],[Draw]], EXP(1))*Table2[[#This Row],[NeitherWon]]</f>
+        <f>-LOG(Table2[[#This Row],[draw]], EXP(1))*Table2[[#This Row],[noteamwins]]</f>
         <v>1.422958345491482</v>
       </c>
       <c r="O11">
@@ -1597,10 +1597,10 @@
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B12" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C12">
         <v>1</v>
@@ -1630,15 +1630,15 @@
         <v>0</v>
       </c>
       <c r="L12">
-        <f>-LOG(Table2[[#This Row],[A Wins]], EXP(1))*Table2[[#This Row],[Awon]]</f>
+        <f>-LOG(Table2[[#This Row],[team1wins]], EXP(1))*Table2[[#This Row],[team1won]]</f>
         <v>0</v>
       </c>
       <c r="M12">
-        <f>-LOG(Table2[[#This Row],[B Wins]], EXP(1))*Table2[[#This Row],[Bwon]]</f>
+        <f>-LOG(Table2[[#This Row],[team2wins]], EXP(1))*Table2[[#This Row],[team2wins2]]</f>
         <v>0.39526728313171838</v>
       </c>
       <c r="N12">
-        <f>-LOG(Table2[[#This Row],[Draw]], EXP(1))*Table2[[#This Row],[NeitherWon]]</f>
+        <f>-LOG(Table2[[#This Row],[draw]], EXP(1))*Table2[[#This Row],[noteamwins]]</f>
         <v>0</v>
       </c>
       <c r="O12">
@@ -1648,10 +1648,10 @@
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B13" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C13">
         <v>1</v>
@@ -1681,15 +1681,15 @@
         <v>0</v>
       </c>
       <c r="L13">
-        <f>-LOG(Table2[[#This Row],[A Wins]], EXP(1))*Table2[[#This Row],[Awon]]</f>
+        <f>-LOG(Table2[[#This Row],[team1wins]], EXP(1))*Table2[[#This Row],[team1won]]</f>
         <v>1.2517634681622845</v>
       </c>
       <c r="M13">
-        <f>-LOG(Table2[[#This Row],[B Wins]], EXP(1))*Table2[[#This Row],[Bwon]]</f>
+        <f>-LOG(Table2[[#This Row],[team2wins]], EXP(1))*Table2[[#This Row],[team2wins2]]</f>
         <v>0</v>
       </c>
       <c r="N13">
-        <f>-LOG(Table2[[#This Row],[Draw]], EXP(1))*Table2[[#This Row],[NeitherWon]]</f>
+        <f>-LOG(Table2[[#This Row],[draw]], EXP(1))*Table2[[#This Row],[noteamwins]]</f>
         <v>0</v>
       </c>
       <c r="O13">

</xml_diff>